<commit_message>
SO fulfillment for single line in VF and LUI mode
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -1,51 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF44932C-AEB8-442C-BB01-0BF0376D099B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BF44932C-AEB8-442C-BB01-0BF0376D099B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="22680" yWindow="795" windowWidth="23850" windowHeight="9285" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" firstSheet="2" windowHeight="9285" windowWidth="23850" xWindow="22680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="795"/>
   </bookViews>
   <sheets>
-    <sheet name="AddHeader" sheetId="14" r:id="rId1"/>
-    <sheet name="AddLine" sheetId="15" r:id="rId2"/>
-    <sheet name="AddLine_Partial" sheetId="19" r:id="rId3"/>
-    <sheet name="InventoryQuantity" sheetId="12" r:id="rId4"/>
-    <sheet name="Account" sheetId="39" r:id="rId5"/>
-    <sheet name="Payments" sheetId="30" r:id="rId6"/>
-    <sheet name="Prepayment" sheetId="37" r:id="rId7"/>
-    <sheet name="OpptyQuote" sheetId="38" r:id="rId8"/>
-    <sheet name="FirmAllLines" sheetId="31" r:id="rId9"/>
-    <sheet name="Allocate" sheetId="32" r:id="rId10"/>
-    <sheet name="PickPackShip" sheetId="33" r:id="rId11"/>
-    <sheet name="CreateInvoice" sheetId="34" r:id="rId12"/>
-    <sheet name="NewInvoice" sheetId="35" r:id="rId13"/>
-    <sheet name="CreditMemo" sheetId="36" r:id="rId14"/>
-    <sheet name="SOFulfillment" sheetId="16" r:id="rId15"/>
-    <sheet name="SOFulfillReverse" sheetId="25" r:id="rId16"/>
-    <sheet name="SOFulfillReverse_Complete" sheetId="27" r:id="rId17"/>
-    <sheet name="Requirements_Complete" sheetId="21" r:id="rId18"/>
-    <sheet name="SOFulfillment_Complete" sheetId="26" r:id="rId19"/>
-    <sheet name="RequirementsAfterPartialReverse" sheetId="22" r:id="rId20"/>
-    <sheet name="ReqAfterReversal_Complete" sheetId="29" r:id="rId21"/>
-    <sheet name="Requirements" sheetId="9" r:id="rId22"/>
-    <sheet name="Requirements_Partial" sheetId="17" r:id="rId23"/>
-    <sheet name="SOORDDMD" sheetId="10" r:id="rId24"/>
-    <sheet name="SOORDDMD_Complete" sheetId="23" r:id="rId25"/>
-    <sheet name="SOORDDMDAfterPartialReverse" sheetId="24" r:id="rId26"/>
-    <sheet name="SOORDDMD_Partial" sheetId="18" r:id="rId27"/>
-    <sheet name="SOORDDMDAfterReversal_Complete" sheetId="28" r:id="rId28"/>
-    <sheet name="Dimensions" sheetId="11" r:id="rId29"/>
+    <sheet name="AddHeader" r:id="rId1" sheetId="14"/>
+    <sheet name="AddLine" r:id="rId2" sheetId="15"/>
+    <sheet name="AddLine_Partial" r:id="rId3" sheetId="19"/>
+    <sheet name="InventoryQuantity" r:id="rId4" sheetId="12"/>
+    <sheet name="Account" r:id="rId5" sheetId="39"/>
+    <sheet name="Payments" r:id="rId6" sheetId="30"/>
+    <sheet name="Prepayment" r:id="rId7" sheetId="37"/>
+    <sheet name="OpptyQuote" r:id="rId8" sheetId="38"/>
+    <sheet name="FirmAllLines" r:id="rId9" sheetId="31"/>
+    <sheet name="Allocate" r:id="rId10" sheetId="32"/>
+    <sheet name="PickPackShip" r:id="rId11" sheetId="33"/>
+    <sheet name="CreateInvoice" r:id="rId12" sheetId="34"/>
+    <sheet name="NewInvoice" r:id="rId13" sheetId="35"/>
+    <sheet name="CreditMemo" r:id="rId14" sheetId="36"/>
+    <sheet name="SOFulfillment" r:id="rId15" sheetId="16"/>
+    <sheet name="SOFulfillReverse" r:id="rId16" sheetId="25"/>
+    <sheet name="SOFulfillReverse_Complete" r:id="rId17" sheetId="27"/>
+    <sheet name="Requirements_Complete" r:id="rId18" sheetId="21"/>
+    <sheet name="SOFulfillment_Complete" r:id="rId19" sheetId="26"/>
+    <sheet name="RequirementsAfterPartialReverse" r:id="rId20" sheetId="22"/>
+    <sheet name="ReqAfterReversal_Complete" r:id="rId21" sheetId="29"/>
+    <sheet name="Requirements" r:id="rId22" sheetId="9"/>
+    <sheet name="Requirements_Partial" r:id="rId23" sheetId="17"/>
+    <sheet name="SOORDDMD" r:id="rId24" sheetId="10"/>
+    <sheet name="SOORDDMD_Complete" r:id="rId25" sheetId="23"/>
+    <sheet name="SOORDDMDAfterPartialReverse" r:id="rId26" sheetId="24"/>
+    <sheet name="SOORDDMD_Partial" r:id="rId27" sheetId="18"/>
+    <sheet name="SOORDDMDAfterReversal_Complete" r:id="rId28" sheetId="28"/>
+    <sheet name="Dimensions" r:id="rId29" sheetId="11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="152">
   <si>
     <t>Customer</t>
   </si>
@@ -506,13 +506,28 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>99117.0</t>
+  </si>
+  <si>
+    <t>99566.0</t>
+  </si>
+  <si>
+    <t>69.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +573,186 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -567,7 +762,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -575,29 +770,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="40">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="1" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="2" fillId="0" fontId="10" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="3" fillId="0" fontId="12" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="4" fillId="0" fontId="14" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="5" fillId="0" fontId="16" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="6" fillId="0" fontId="18" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="7" fillId="0" fontId="20" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="8" fillId="0" fontId="22" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="24" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="25" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="26" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="28" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="29" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="30" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="31" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="32" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="33" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="34" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="15" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -614,10 +884,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -652,7 +922,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -687,7 +957,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -781,21 +1051,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -812,7 +1082,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -864,14 +1134,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28DC5EA-FDB2-4037-A650-5A7807A76B42}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28DC5EA-FDB2-4037-A650-5A7807A76B42}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -880,13 +1150,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,12 +1212,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E5A5D2-ADF8-4D4A-A3A2-BBBA14DE25A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E5A5D2-ADF8-4D4A-A3A2-BBBA14DE25A1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -956,9 +1226,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,12 +1254,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F66068-E890-47C4-8EBD-0950A83EA35F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F66068-E890-47C4-8EBD-0950A83EA35F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -998,7 +1268,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,12 +1294,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC5F489-EACC-4914-ABCD-2F1E7C8D2169}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC5F489-EACC-4914-ABCD-2F1E7C8D2169}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1038,7 +1308,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,12 +1334,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2009802-983D-44C0-AB88-E82E300B78E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2009802-983D-44C0-AB88-E82E300B78E3}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1078,11 +1348,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,14 +1391,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" xr:uid="{9745F9A5-F47A-42F2-8FA4-C71F817D0139}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" r:id="rId1" ref="A2" xr:uid="{9745F9A5-F47A-42F2-8FA4-C71F817D0139}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B74EF4C-3342-4EE1-8981-E671C6C95E50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B74EF4C-3342-4EE1-8981-E671C6C95E50}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1137,8 +1407,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,14 +1447,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" xr:uid="{2B6F5591-69D6-4870-A951-0F09FF95F53E}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" r:id="rId1" ref="B2" xr:uid="{2B6F5591-69D6-4870-A951-0F09FF95F53E}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E98237-5B33-4FA7-92DA-167DD1319B66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E98237-5B33-4FA7-92DA-167DD1319B66}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1193,8 +1463,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1252,12 +1522,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DBE7BB-BE32-4604-BF8E-2DC6649FEFD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DBE7BB-BE32-4604-BF8E-2DC6649FEFD0}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1351,12 +1621,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA16FCEB-84ED-4ADE-A0CB-36816265E5E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA16FCEB-84ED-4ADE-A0CB-36816265E5E8}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1365,8 +1635,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1436,12 +1706,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127F6FBD-E0D5-47A3-9477-A6E957539DB5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127F6FBD-E0D5-47A3-9477-A6E957539DB5}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1450,11 +1720,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1526,12 +1796,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C42A8B7-E8CA-4808-B9C2-F08D9DD12C52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C42A8B7-E8CA-4808-B9C2-F08D9DD12C52}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1540,8 +1810,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1593,12 +1863,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513CC44F-3165-4623-A12A-9D782A7314E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513CC44F-3165-4623-A12A-9D782A7314E2}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -1607,18 +1877,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1856,13 +2126,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62A9229-E86A-4027-BB56-A44835B7F72B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62A9229-E86A-4027-BB56-A44835B7F72B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1871,11 +2141,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1930,12 +2200,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA4FCB4-E35D-4534-B2C1-E70F12719CC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA4FCB4-E35D-4534-B2C1-E70F12719CC8}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1944,11 +2214,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2003,12 +2273,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C60F850-BC07-45D7-8A71-F5FA33E22AE5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C60F850-BC07-45D7-8A71-F5FA33E22AE5}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2017,11 +2287,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2093,12 +2363,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A560793F-0494-4CD5-BC3A-BDC8EE3E00DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A560793F-0494-4CD5-BC3A-BDC8EE3E00DA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2107,11 +2377,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2183,12 +2453,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8A9A71-0839-422E-A3E9-10597D3A681D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8A9A71-0839-422E-A3E9-10597D3A681D}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2197,11 +2467,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2273,12 +2543,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC13E90-A910-4F2B-A97F-391C58C0C01E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC13E90-A910-4F2B-A97F-391C58C0C01E}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2287,9 +2557,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2362,16 +2632,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syri?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVO%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000QgsQ%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" xr:uid="{3F87EA66-600E-442E-A623-C5F51524DC7D}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrn?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVT%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000Qgsa%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" xr:uid="{EAAA2D23-76D0-491A-AC97-347EF698B431}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrs?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVn%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsopcomp%253FactionType%253Dview%2526id%253Da661K000000HCf3QAG" xr:uid="{47001F2F-B95D-42AC-BADD-D4214A1FE5E0}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syri?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVO%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000QgsQ%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" r:id="rId1" ref="B2" xr:uid="{3F87EA66-600E-442E-A623-C5F51524DC7D}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrn?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVT%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000Qgsa%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" r:id="rId2" ref="B3" xr:uid="{EAAA2D23-76D0-491A-AC97-347EF698B431}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrs?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVn%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsopcomp%253FactionType%253Dview%2526id%253Da661K000000HCf3QAG" r:id="rId3" ref="B4" xr:uid="{47001F2F-B95D-42AC-BADD-D4214A1FE5E0}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B33A50A-62EE-4A11-9018-AC7DAE1E9EBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B33A50A-62EE-4A11-9018-AC7DAE1E9EBF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2380,9 +2650,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2455,16 +2725,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syri?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVO%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000QgsQ%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" xr:uid="{2B9DD9C4-9669-4450-92C7-9867560E2E1E}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrn?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVT%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000Qgsa%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" xr:uid="{D006B536-37C0-4EA2-AE82-33D3E8C9FEE4}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrs?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVn%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsopcomp%253FactionType%253Dview%2526id%253Da661K000000HCf3QAG" xr:uid="{F224F8C3-F4BE-4A1A-A718-97F57505E1AC}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syri?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVO%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000QgsQ%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" r:id="rId1" ref="B2" xr:uid="{2B9DD9C4-9669-4450-92C7-9867560E2E1E}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrn?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVT%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000Qgsa%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" r:id="rId2" ref="B3" xr:uid="{D006B536-37C0-4EA2-AE82-33D3E8C9FEE4}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrs?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVn%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsopcomp%253FactionType%253Dview%2526id%253Da661K000000HCf3QAG" r:id="rId3" ref="B4" xr:uid="{F224F8C3-F4BE-4A1A-A718-97F57505E1AC}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44C4694-381A-4457-8D8C-ADD3CA0E5F41}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44C4694-381A-4457-8D8C-ADD3CA0E5F41}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2473,9 +2743,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2547,12 +2817,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0933D21E-089C-4C90-9CAD-0DFCF820E07F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0933D21E-089C-4C90-9CAD-0DFCF820E07F}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2561,9 +2831,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,16 +2906,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syri?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVO%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000QgsQ%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" xr:uid="{EB85B907-E74C-4DD6-B294-57DA732C1E64}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrn?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVT%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000Qgsa%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" xr:uid="{3C06B6DD-07FF-42BA-873D-A9AA6109627A}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrs?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVn%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsopcomp%253FactionType%253Dview%2526id%253Da661K000000HCf3QAG" xr:uid="{8E3099A3-1F53-4FA3-BBA9-F2C2B1952F16}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syri?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVO%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000QgsQ%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" r:id="rId1" ref="B2" xr:uid="{EB85B907-E74C-4DD6-B294-57DA732C1E64}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrn?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVT%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsoprod%253FactionType%253Dview%2526id%253Da6J1K000000Qgsa%2526returnURL%253Dhttps%25253A%25252F%25252Frstk-qa-rsf--rstk.na75.visual.force.com%25252Fapex%25252FSalesOrder%25253Fid%25253Da5P1K000001kh5b%252526sfdc.override%25253D1" r:id="rId2" ref="B3" xr:uid="{3C06B6DD-07FF-42BA-873D-A9AA6109627A}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a2S1K000002Syrs?returnURL=https%3A//rstk-qa-rsf--rstk.na75.visual.force.com/apex/icitem%3FactionType%3Dview%26id%3Da1E1K000009KCVn%26returnURL%3Dhttps%253A%252F%252Frstk-qa-rsf--rstk.na75.visual.force.com%252Fapex%252Fsopcomp%253FactionType%253Dview%2526id%253Da661K000000HCf3QAG" r:id="rId3" ref="B4" xr:uid="{8E3099A3-1F53-4FA3-BBA9-F2C2B1952F16}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F9AC43-F5C0-448B-A649-9DBCCD7B9161}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F9AC43-F5C0-448B-A649-9DBCCD7B9161}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -2654,14 +2924,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="49.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="49.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2798,12 +3068,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F745D4BD-94B9-4920-AF2D-A59E170DB0E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F745D4BD-94B9-4920-AF2D-A59E170DB0E2}">
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2812,17 +3082,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3042,12 +3312,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7667096-5FA7-42EB-ACDF-85A64908BEC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7667096-5FA7-42EB-ACDF-85A64908BEC3}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3056,10 +3326,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.83984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.3984375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.97265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3081,7 +3351,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -3095,7 +3365,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>134</v>
@@ -3109,7 +3379,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>135</v>
@@ -3120,13 +3390,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7C87B-7082-49FA-9A1A-6F0FEB2DF64F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7C87B-7082-49FA-9A1A-6F0FEB2DF64F}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3135,12 +3405,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3196,12 +3466,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7584A231-ABFC-431D-8B43-685A3F1BAAE9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7584A231-ABFC-431D-8B43-685A3F1BAAE9}">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3210,9 +3480,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -3310,12 +3580,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7F51EF-7ECF-434F-A1BE-BA15C47E91C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7F51EF-7ECF-434F-A1BE-BA15C47E91C0}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3324,8 +3594,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3376,16 +3646,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" xr:uid="{71C4F047-1237-4195-ACFF-51598D5DF40F}"/>
-    <hyperlink ref="F2" r:id="rId2" display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" xr:uid="{F099F36E-E43B-4BF9-8B75-98C3EB6188DC}"/>
-    <hyperlink ref="G2" r:id="rId3" display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" xr:uid="{8A570B2E-944A-4708-BC66-1FD9ECDA8E25}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" r:id="rId1" ref="C2" xr:uid="{71C4F047-1237-4195-ACFF-51598D5DF40F}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" r:id="rId2" ref="F2" xr:uid="{F099F36E-E43B-4BF9-8B75-98C3EB6188DC}"/>
+    <hyperlink display="https://rstk-qa-rsf.my.salesforce.com/a6J1K000000Qgsa" r:id="rId3" ref="G2" xr:uid="{8A570B2E-944A-4708-BC66-1FD9ECDA8E25}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42723DB2-2BC3-4244-AAEC-76056E050AD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42723DB2-2BC3-4244-AAEC-76056E050AD6}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3394,8 +3664,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3453,12 +3723,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715F1D47-B4B0-4D87-973F-66E59D325D07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715F1D47-B4B0-4D87-973F-66E59D325D07}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3467,8 +3737,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3489,6 +3759,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated SO Test Cases
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{BF44932C-AEB8-442C-BB01-0BF0376D099B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{4221CF31-DDDA-40AF-8D49-4D2FF3B86499}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="2" windowHeight="9285" windowWidth="23850" xWindow="22680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="795"/>
+    <workbookView activeTab="3" windowHeight="10920" windowWidth="26670" xWindow="21525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="5265"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" r:id="rId1" sheetId="14"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="185">
   <si>
     <t>Customer</t>
   </si>
@@ -454,15 +454,6 @@
     <t>PB_Automation</t>
   </si>
   <si>
-    <t>55.0</t>
-  </si>
-  <si>
-    <t>99617.0</t>
-  </si>
-  <si>
-    <t>99814.0</t>
-  </si>
-  <si>
     <t>53.0</t>
   </si>
   <si>
@@ -508,16 +499,124 @@
     <t>India</t>
   </si>
   <si>
-    <t>70.0</t>
-  </si>
-  <si>
-    <t>99117.0</t>
-  </si>
-  <si>
-    <t>99566.0</t>
-  </si>
-  <si>
-    <t>69.0</t>
+    <t>54.0</t>
+  </si>
+  <si>
+    <t>99107.0</t>
+  </si>
+  <si>
+    <t>99560.0</t>
+  </si>
+  <si>
+    <t>DiscountPct</t>
+  </si>
+  <si>
+    <t>52.0</t>
+  </si>
+  <si>
+    <t>99105.0</t>
+  </si>
+  <si>
+    <t>99558.0</t>
+  </si>
+  <si>
+    <t>51.0</t>
+  </si>
+  <si>
+    <t>99103.0</t>
+  </si>
+  <si>
+    <t>99557.0</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>99101.0</t>
+  </si>
+  <si>
+    <t>99556.0</t>
+  </si>
+  <si>
+    <t>49.0</t>
+  </si>
+  <si>
+    <t>99099.0</t>
+  </si>
+  <si>
+    <t>99555.0</t>
+  </si>
+  <si>
+    <t>48.0</t>
+  </si>
+  <si>
+    <t>99097.0</t>
+  </si>
+  <si>
+    <t>99554.0</t>
+  </si>
+  <si>
+    <t>47.0</t>
+  </si>
+  <si>
+    <t>99095.0</t>
+  </si>
+  <si>
+    <t>99553.0</t>
+  </si>
+  <si>
+    <t>41.0</t>
+  </si>
+  <si>
+    <t>99087.0</t>
+  </si>
+  <si>
+    <t>99547.0</t>
+  </si>
+  <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>99077.0</t>
+  </si>
+  <si>
+    <t>99542.0</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>99075.0</t>
+  </si>
+  <si>
+    <t>99541.0</t>
+  </si>
+  <si>
+    <t>34.0</t>
+  </si>
+  <si>
+    <t>99073.0</t>
+  </si>
+  <si>
+    <t>99540.0</t>
+  </si>
+  <si>
+    <t>31.0</t>
+  </si>
+  <si>
+    <t>99067.0</t>
+  </si>
+  <si>
+    <t>99537.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>99065.0</t>
+  </si>
+  <si>
+    <t>99536.0</t>
   </si>
 </sst>
 </file>
@@ -527,7 +626,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="163" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,6 +671,762 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -762,7 +1617,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="79">
     <border>
       <left/>
       <right/>
@@ -815,11 +1670,200 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="166">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -860,8 +1904,134 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="32" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="33" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="14" fillId="0" fontId="34" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="15" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="35" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="15" fillId="0" fontId="36" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="37" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="38" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="40" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="42" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="43" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="44" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="45" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="46" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="48" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="49" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="50" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="51" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="52" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="53" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="54" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="55" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="56" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="57" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="58" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="59" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="60" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="61" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="62" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="63" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="29" fillId="0" fontId="64" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="65" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="66" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="67" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="68" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="69" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="70" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="71" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="72" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="73" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="74" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="75" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="76" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="77" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="36" fillId="0" fontId="78" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="79" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="80" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="81" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="82" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="83" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="84" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="85" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="86" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="87" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="88" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="89" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="90" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="91" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="92" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="93" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="94" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="95" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="96" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="97" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="98" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="99" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="100" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="101" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="102" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="103" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="104" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="105" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="106" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="107" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="108" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="109" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="110" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="111" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="112" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="113" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="114" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="115" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="116" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="117" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="118" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="119" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="120" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="121" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="122" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="123" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="124" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="125" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="126" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="127" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="128" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="129" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="130" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="131" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="132" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="133" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="134" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="135" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="136" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="137" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="138" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="139" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="140" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="141" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="68" fillId="0" fontId="142" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="143" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="69" fillId="0" fontId="144" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="145" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="70" fillId="0" fontId="146" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="147" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="148" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="149" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="72" fillId="0" fontId="150" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="151" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="73" fillId="0" fontId="152" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="153" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="74" fillId="0" fontId="154" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="155" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="75" fillId="0" fontId="156" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="157" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="76" fillId="0" fontId="158" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="159" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="77" fillId="0" fontId="160" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="162" fillId="0" borderId="78" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1869,10 +3039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513CC44F-3165-4623-A12A-9D782A7314E2}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,12 +3056,13 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="29.7109375" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1923,16 +3094,19 @@
         <v>2</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1964,16 +3138,19 @@
         <v>200</v>
       </c>
       <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -2005,13 +3182,16 @@
         <v>100</v>
       </c>
       <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -2043,13 +3223,16 @@
         <v>50</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>3</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -2081,13 +3264,16 @@
         <v>80</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>4</v>
       </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -2119,9 +3305,12 @@
         <v>20</v>
       </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>5</v>
       </c>
-      <c r="L6" t="b">
+      <c r="M6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3351,10 +4540,10 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3365,10 +4554,10 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3379,10 +4568,10 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3399,8 +4588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F7C87B-7082-49FA-9A1A-6F0FEB2DF64F}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3415,28 +4604,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,19 +4636,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F2">
         <v>411038</v>
       </c>
       <c r="G2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H2">
         <v>1236547891</v>

</xml_diff>

<commit_message>
Updated SO test cases where callables were missing
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="187">
   <si>
     <t>Customer</t>
   </si>
@@ -617,6 +617,12 @@
   </si>
   <si>
     <t>99536.0</t>
+  </si>
+  <si>
+    <t>98933.0</t>
+  </si>
+  <si>
+    <t>99475.0</t>
   </si>
 </sst>
 </file>
@@ -626,7 +632,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="163" x14ac:knownFonts="1">
+  <fonts count="175" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,6 +677,78 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1617,7 +1695,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="79">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -1859,11 +1937,29 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="178">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -2030,8 +2126,20 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="76" fillId="0" fontId="158" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="159" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="77" fillId="0" fontId="160" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="161" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="162" fillId="0" borderId="78" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="161" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="78" fillId="0" fontId="162" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="163" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="79" fillId="0" fontId="164" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="165" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="80" fillId="0" fontId="166" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="167" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="81" fillId="0" fontId="168" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="169" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="82" fillId="0" fontId="170" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="171" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="83" fillId="0" fontId="172" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="174" fillId="0" borderId="84" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4540,7 +4648,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
@@ -4554,7 +4662,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>165</v>
@@ -4568,7 +4676,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
Updated SO UI TCs, Renamed SYDATA TCs with their Jira Numbers
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3AEE612F-D20D-4380-B129-7863B454B0FA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{349E109C-6687-4857-9F49-5867572EC020}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="15" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" r:id="rId1" sheetId="14"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="161">
   <si>
     <t>Customer</t>
   </si>
@@ -494,60 +494,6 @@
     <t>DiscountPct</t>
   </si>
   <si>
-    <t>71.0</t>
-  </si>
-  <si>
-    <t>97406.0</t>
-  </si>
-  <si>
-    <t>98702.0</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
-    <t>97402.0</t>
-  </si>
-  <si>
-    <t>98700.0</t>
-  </si>
-  <si>
-    <t>70.0</t>
-  </si>
-  <si>
-    <t>97404.0</t>
-  </si>
-  <si>
-    <t>98701.0</t>
-  </si>
-  <si>
-    <t>68.0</t>
-  </si>
-  <si>
-    <t>97400.0</t>
-  </si>
-  <si>
-    <t>98699.0</t>
-  </si>
-  <si>
-    <t>67.0</t>
-  </si>
-  <si>
-    <t>97398.0</t>
-  </si>
-  <si>
-    <t>98698.0</t>
-  </si>
-  <si>
-    <t>75.0</t>
-  </si>
-  <si>
-    <t>97313.0</t>
-  </si>
-  <si>
-    <t>98656.0</t>
-  </si>
-  <si>
     <t>74.0</t>
   </si>
   <si>
@@ -555,6 +501,51 @@
   </si>
   <si>
     <t>98655.0</t>
+  </si>
+  <si>
+    <t>39.0</t>
+  </si>
+  <si>
+    <t>97241.0</t>
+  </si>
+  <si>
+    <t>98620.0</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>97239.0</t>
+  </si>
+  <si>
+    <t>98619.0</t>
+  </si>
+  <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>97235.0</t>
+  </si>
+  <si>
+    <t>98617.0</t>
+  </si>
+  <si>
+    <t>37.0</t>
+  </si>
+  <si>
+    <t>97237.0</t>
+  </si>
+  <si>
+    <t>98618.0</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>97233.0</t>
+  </si>
+  <si>
+    <t>98616.0</t>
   </si>
 </sst>
 </file>
@@ -564,7 +555,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="79" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,222 +600,6 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="10.0"/>
-      <color indexed="10"/>
-      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1051,7 +826,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1113,65 +888,11 @@
     <border>
       <bottom style="thin"/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1218,44 +939,8 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="16" fillId="0" fontId="38" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="17" fillId="0" fontId="40" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="18" fillId="0" fontId="42" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="43" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="19" fillId="0" fontId="44" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="45" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="20" fillId="0" fontId="46" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="21" fillId="0" fontId="48" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="49" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="22" fillId="0" fontId="50" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="51" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="23" fillId="0" fontId="52" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="53" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="24" fillId="0" fontId="54" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="55" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="25" fillId="0" fontId="56" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="57" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="26" fillId="0" fontId="58" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="59" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="27" fillId="0" fontId="60" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="61" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="28" fillId="0" fontId="62" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="63" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="29" fillId="0" fontId="64" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="65" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="30" fillId="0" fontId="66" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="67" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="31" fillId="0" fontId="68" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="69" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="32" fillId="0" fontId="70" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="71" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="33" fillId="0" fontId="72" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="73" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="34" fillId="0" fontId="74" numFmtId="49" xfId="0"/>
-    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="75" numFmtId="164" xfId="0"/>
-    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="35" fillId="0" fontId="76" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="78" fillId="0" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="18" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2198,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EBB0E8-7736-4B3E-8E32-A499FC9E511B}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,7 +1951,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="H1" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,10 +3081,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F745D4BD-94B9-4920-AF2D-A59E170DB0E2}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,14 +3095,15 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -3440,22 +3126,25 @@
         <v>1</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -3477,23 +3166,26 @@
       <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -3515,20 +3207,23 @@
       <c r="G3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -3550,20 +3245,23 @@
       <c r="G4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -3585,20 +3283,23 @@
       <c r="G5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>80</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -3620,16 +3321,19 @@
       <c r="G6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5</v>
       </c>
-      <c r="K6" t="b">
+      <c r="L6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3831,10 +3535,10 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3845,10 +3549,10 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3859,10 +3563,10 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>

<commit_message>
SO -Updated Folder Name for Callable TCs.
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="198">
   <si>
     <t>Customer</t>
   </si>
@@ -579,6 +579,84 @@
   </si>
   <si>
     <t>98613.0</t>
+  </si>
+  <si>
+    <t>97054.0</t>
+  </si>
+  <si>
+    <t>98527.0</t>
+  </si>
+  <si>
+    <t>128.0</t>
+  </si>
+  <si>
+    <t>97045.0</t>
+  </si>
+  <si>
+    <t>98523.0</t>
+  </si>
+  <si>
+    <t>127.0</t>
+  </si>
+  <si>
+    <t>97043.0</t>
+  </si>
+  <si>
+    <t>98522.0</t>
+  </si>
+  <si>
+    <t>126.0</t>
+  </si>
+  <si>
+    <t>97041.0</t>
+  </si>
+  <si>
+    <t>98521.0</t>
+  </si>
+  <si>
+    <t>125.0</t>
+  </si>
+  <si>
+    <t>97039.0</t>
+  </si>
+  <si>
+    <t>98520.0</t>
+  </si>
+  <si>
+    <t>124.0</t>
+  </si>
+  <si>
+    <t>97037.0</t>
+  </si>
+  <si>
+    <t>98519.0</t>
+  </si>
+  <si>
+    <t>122.0</t>
+  </si>
+  <si>
+    <t>97033.0</t>
+  </si>
+  <si>
+    <t>98517.0</t>
+  </si>
+  <si>
+    <t>123.0</t>
+  </si>
+  <si>
+    <t>97035.0</t>
+  </si>
+  <si>
+    <t>98518.0</t>
+  </si>
+  <si>
+    <t>121.0</t>
+  </si>
+  <si>
+    <t>97031.0</t>
+  </si>
+  <si>
+    <t>98516.0</t>
   </si>
 </sst>
 </file>
@@ -588,7 +666,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="85" x14ac:knownFonts="1">
+  <fonts count="187" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,6 +711,618 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1111,7 +1801,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="91">
     <border>
       <left/>
       <right/>
@@ -1236,11 +1926,164 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="190">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -1329,8 +2172,110 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="37" fillId="0" fontId="80" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="81" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="38" fillId="0" fontId="82" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="84" fillId="0" borderId="39" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="83" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="39" fillId="0" fontId="84" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="85" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="40" fillId="0" fontId="86" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="87" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="41" fillId="0" fontId="88" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="89" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="42" fillId="0" fontId="90" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="91" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="43" fillId="0" fontId="92" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="93" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="44" fillId="0" fontId="94" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="95" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="45" fillId="0" fontId="96" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="97" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="46" fillId="0" fontId="98" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="99" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="47" fillId="0" fontId="100" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="101" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="48" fillId="0" fontId="102" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="103" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="49" fillId="0" fontId="104" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="105" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="50" fillId="0" fontId="106" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="107" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="51" fillId="0" fontId="108" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="109" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="52" fillId="0" fontId="110" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="111" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="53" fillId="0" fontId="112" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="113" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="54" fillId="0" fontId="114" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="115" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="55" fillId="0" fontId="116" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="117" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="56" fillId="0" fontId="118" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="119" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="57" fillId="0" fontId="120" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="121" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="58" fillId="0" fontId="122" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="123" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="59" fillId="0" fontId="124" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="125" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="60" fillId="0" fontId="126" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="127" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="61" fillId="0" fontId="128" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="129" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="62" fillId="0" fontId="130" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="131" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="63" fillId="0" fontId="132" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="133" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="64" fillId="0" fontId="134" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="135" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="65" fillId="0" fontId="136" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="137" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="66" fillId="0" fontId="138" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="139" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="67" fillId="0" fontId="140" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="141" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="68" fillId="0" fontId="142" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="143" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="69" fillId="0" fontId="144" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="145" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="70" fillId="0" fontId="146" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="147" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="71" fillId="0" fontId="148" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="149" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="72" fillId="0" fontId="150" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="151" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="73" fillId="0" fontId="152" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="153" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="74" fillId="0" fontId="154" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="155" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="75" fillId="0" fontId="156" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="157" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="76" fillId="0" fontId="158" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="159" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="77" fillId="0" fontId="160" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="161" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="78" fillId="0" fontId="162" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="163" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="79" fillId="0" fontId="164" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="165" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="80" fillId="0" fontId="166" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="167" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="81" fillId="0" fontId="168" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="169" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="82" fillId="0" fontId="170" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="171" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="83" fillId="0" fontId="172" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="173" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="84" fillId="0" fontId="174" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="175" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="85" fillId="0" fontId="176" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="177" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="86" fillId="0" fontId="178" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="179" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="87" fillId="0" fontId="180" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="181" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="88" fillId="0" fontId="182" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="183" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="89" fillId="0" fontId="184" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="186" fillId="0" borderId="90" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3925,10 +4870,10 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3939,10 +4884,10 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -3953,10 +4898,10 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>

<commit_message>
Added testcases for Newly added SYDATA Transactions|Change in test Plan folder structure-Inventory Transactions
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
+++ b/templates/AutomationOrg/SalesOrder_BaseData_SOAPI.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="217">
   <si>
     <t>Customer</t>
   </si>
@@ -697,6 +697,24 @@
   </si>
   <si>
     <t>97875.0</t>
+  </si>
+  <si>
+    <t>145.0</t>
+  </si>
+  <si>
+    <t>95733.0</t>
+  </si>
+  <si>
+    <t>97873.0</t>
+  </si>
+  <si>
+    <t>141.0</t>
+  </si>
+  <si>
+    <t>95725.0</t>
+  </si>
+  <si>
+    <t>97869.0</t>
   </si>
 </sst>
 </file>
@@ -706,7 +724,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="175" x14ac:knownFonts="1">
+  <fonts count="187" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,6 +769,78 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1769,7 +1859,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="85">
+  <borders count="91">
     <border>
       <left/>
       <right/>
@@ -2029,11 +2119,29 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="190">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -2212,8 +2320,20 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="82" fillId="0" fontId="170" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="171" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="83" fillId="0" fontId="172" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="173" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="174" fillId="0" borderId="84" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="173" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="84" fillId="0" fontId="174" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="175" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="85" fillId="0" fontId="176" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="177" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="86" fillId="0" fontId="178" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="179" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="87" fillId="0" fontId="180" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="181" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="88" fillId="0" fontId="182" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="183" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="89" fillId="0" fontId="184" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="186" fillId="0" borderId="90" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4849,7 +4969,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
         <v>208</v>
@@ -4863,7 +4983,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>209</v>
@@ -4877,7 +4997,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="C4" t="s">
         <v>210</v>

</xml_diff>